<commit_message>
Update all paper links
</commit_message>
<xml_diff>
--- a/CV/Papers.xlsx
+++ b/CV/Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltraeger/MyAcademicSite/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FBCD0C-F1AE-684C-9F2A-D4896BD8AC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B0DA86-BA81-234D-B1D8-47EBDD7DFBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="-6360" windowWidth="51200" windowHeight="28300" xr2:uid="{70AAFC3F-B0F4-DE41-8EF2-4D6A666AD290}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="278">
   <si>
     <t>Nevendorrf L, Pedrana A, Bourne A, Traeger M, Sindunata E, Reswana WA, Alharbi RM, Stoové M. Characterizing socioecological markers of differentiated HIV risk among men who have sex with men in Indonesia. AIDS and Behavior. Online 25 Jan 2024. doi:10.1007/s10461-023-04253-3</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Cornelisse VJ, Murphy D, Lee SJ, Stoove M, **Traeger MW**, Wright EJ. Physical and mental health of long-term users of HIV pre-exposure prophylaxis (PrEP) in Australia: The X-PLORE Cohort. AIDS. Online 26 Oct 2023. doi:10.1097/QAD.0000000000003678</t>
   </si>
   <si>
-    <t>Munari SC*, **Traeger MW***, Menon V, Latham NH, Manoharan L, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Conway B, Klein M, Bruneau J, Stoové MA, Hellard ME, Doyle JS. Determining reinfection rates by hepatitis C testing interval among key populations: a systematic review and meta-analysis. Online 10 Oct 2023. doi:10.1111/liv.15705</t>
-  </si>
-  <si>
     <t>Mayer KH, **Traeger MW**, Marcus JL. Doxycycline Postexposure Prophylaxis and Sexually Transmitted Infections. Journal of the American Medical Association. Online 22 Sep 2023. doi:10.1001/jama.2023.16416</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>Wilkinson AL, van Santen DK, **Traeger MW**, Sacks-Davis R, Asselin J, Scott N, Harney B, Doyle JS, El-Hayek C, Howell J, Bramwell F, McManus H, Donovan B, Guy R, Stoové M, Hellard M, Pedrana A. Hepatitis C incidence among patients attending primary care health services that specialise in the care of people who inject drugs, Victoria, Australia, 2009 to 2020. International Journal of Drug Policy. 2022Mar 25;103:103655. doi:10.1016/j.drugpo.2022.103655</t>
   </si>
   <si>
-    <t>Howell J, **Traeger MW**, Williams B, Layton C, Doyle J, Latham N, Draper B, Bramwell F, Membrey D, McPherson M, Stoové M, Roney J, Thompson A, Hellard M, Pedrana A. Point-of-care hepatitis C testing in needle and syringe exchange programs increases linkage to care and treatment uptake among people who inject drugs: An Australian pilot study. Journal of Viral Hepatitis. 2022;29:275-384. doi:10.1111/jvh.13664</t>
-  </si>
-  <si>
     <t>Wilkinson AL, Pedrana A, **Traeger MW**, Asselin J, El-Hayek C, Nguyen L, Polkinghorne V, Doyle JS, Thompson AJ, Howell J, Scott N, Dimech W, Guy R, Stoové M, Hellard M. Real world monitoring progress towards the elimination of hepatitis C virus in Australia using sentinel surveillance of primary care clinics: an ecological study of hepatitis C virus antibody tests from 2009 to 2019. Epidemiology and infection. 2021 Dec 6;150:e7. doi:10.1017/S0950268821002624</t>
   </si>
   <si>
@@ -339,9 +333,6 @@
     <t>**Traeger MW**, Patel P, Guy R, Hellard M, Stoové M. Changes in HIV pre-exposure prophylaxis prescribing in Australian clinical services following COVID-10 restrictions. AIDS. 2021;35(1):155-157. doi:10.1097/QAD.0000000000002703</t>
   </si>
   <si>
-    <t>Mwaturura C, **Traeger MW**, Lemoh C, Stoové M, Price B, Coelho A, Mikola M, Ryan K, Wright E. Acceptability, Willingness to Use, Barriers and Facilitators to Pre-exposure Prophylaxis (PrEP) among African Migrants in High-Income Countries: A Systematic Review. Sexual Health. 2021;18(2):130-139. doi: 10.1071/SH20175</t>
-  </si>
-  <si>
     <t>**Traeger MW**, Tidhar T, Holt M, Williams C, Wright E, Stoové M, Scott N, Hellard M. The Potential Impact of a Gel-based Point-of-sex Intervention in Reducing Gonorrhoea Incidence among Gay and Bisexual Men: a Modelling Study. Sexually Transmitted Diseases. 2020; 47(10): 649-657. doi:10.1097/OLQ.0000000000001239</t>
   </si>
   <si>
@@ -456,9 +447,6 @@
     <t>**Traeger M**, Asselin J, Price B, Roth N, Willcox J, Tee BK, Fairley C, Penn M, El-Hayek C, Nguyen L, Ryan K, Hoy J, Ruth S, West M, Stoové M, Wright E. Longitudinal changes in condom use with casual partners among gay and bisexual men using HIV pre-exposure prophylaxis. Australasian HIV&amp;AIDS and Sexual Health Conferences, Perth, Australia. 16-19 September 2019.</t>
   </si>
   <si>
-    <t xml:space="preserve">26. **Traeger M**, Asselin J, Ryan K, Doyle J, Harney B, Pedrana A, El-Hayek C, </t>
-  </si>
-  <si>
     <t>**Traeger M**, Asselin J, Price B, Roth N, Willcox J, Tee BK, Fairley C, Penn M, El-Hayek C, Nguyen L, Ryan K, Hoy J, Ruth S, West M, Stoové M, Wright E. Longitudinal changes in condom use with casual partners among gay and bisexual men using HIV pre-exposure prophylaxis. 10th IAS Conference on HIV Science, Mexico City, Mexico. 21-24 July 2019.</t>
   </si>
   <si>
@@ -658,6 +646,231 @@
   </si>
   <si>
     <t>**Traeger MW**, Stoové MA. Why risk matter for STI control: who are those at greatest risk and how are they identified? Sexual Health. Accepted 26 Apr 2022</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ofid/article/12/2/ofaf056/7998417?login=false</t>
+  </si>
+  <si>
+    <t>Matthews_OFID_2025.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0955395924002469?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Shen_IJDP_2024.pdf</t>
+  </si>
+  <si>
+    <t>**Traeger M**, Asselin J, Ryan K, Doyle J, Harney B, Pedrana A, El-Hayek C, Nguyen L, Roth N, Fairley C, Willcox J, Tee BK, Guy R, Wright E, Hellard M, Stoové. Adherence to Hepatitis C testing guidelines among Victorian gay and bisexual men using HIV pre-exposure prophylaxis. Australasian HIV&amp;AIDS and Sexual Health Conferences, Perth, Australia. 16-19 September 2019.</t>
+  </si>
+  <si>
+    <t>https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(24)00213-3/abstract</t>
+  </si>
+  <si>
+    <t>https://www.thelancet.com/journals/lanwpc/article/PIIS2666-6065(24)00169-X/fulltext</t>
+  </si>
+  <si>
+    <t>Traeger_LancetRHWP_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://sti.bmj.com/content/100/5/295.long</t>
+  </si>
+  <si>
+    <t>Harney_STI_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/stdjournal/fulltext/2024/12000/use_of_doxycycline_and_other_antibiotics_as.1.aspx</t>
+  </si>
+  <si>
+    <t>Traeger_STDs_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://linkinghub.elsevier.com/retrieve/pii/S2589-5370(24)00068-3</t>
+  </si>
+  <si>
+    <t>Hayes_cClinMed_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ofid/article/11/4/ofae099/7610685</t>
+  </si>
+  <si>
+    <t>Harney_OFID_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/liv.15841</t>
+  </si>
+  <si>
+    <t>Harney_LiverInt_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10461-023-04253-3</t>
+  </si>
+  <si>
+    <t>Nevendorrf_AIDSBeh_2024.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/stdjournal/fulltext/2023/12000/trends_in_testing_and_self_reported_diagnoses_of.3.aspx</t>
+  </si>
+  <si>
+    <t>Chan_STDs_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/aidsonline/abstract/2024/03010/physical_and_mental_health_of_long_term_users_of.10.aspx</t>
+  </si>
+  <si>
+    <t>Cornelisse_AIDS_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/liv.15705</t>
+  </si>
+  <si>
+    <t>Munari_LiverInt_2023.pdf</t>
+  </si>
+  <si>
+    <t>Munari SC (co-first), **Traeger MW (co-first)**, Menon V, Latham NH, Manoharan L, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Conway B, Klein M, Bruneau J, Stoové MA, Hellard ME, Doyle JS. Determining reinfection rates by hepatitis C testing interval among key populations: a systematic review and meta-analysis. Online 10 Oct 2023. doi:10.1111/liv.15705</t>
+  </si>
+  <si>
+    <t>https://jamanetwork.com/journals/jama/fullarticle/2810020</t>
+  </si>
+  <si>
+    <t>Mayer_JAMA_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/cid/advance-article/doi/10.1093/cid/ciad488/7245976</t>
+  </si>
+  <si>
+    <t>Traeger_CID_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(23)00171-6/abstract</t>
+  </si>
+  <si>
+    <t>Traeger_LancetHIV_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ofid/article/10/8/ofad401/7234598</t>
+  </si>
+  <si>
+    <t>Traeger_OFID_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/hepcomm/fulltext/2023/04010/immediate_treatment_for_recent_hepatitis_c.2.aspx</t>
+  </si>
+  <si>
+    <t>Manoharan_HepComm_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/jvh.13723</t>
+  </si>
+  <si>
+    <t>Traeger_JVHep_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://linkinghub.elsevier.com/retrieve/pii/S1473-3099(22)00175-X</t>
+  </si>
+  <si>
+    <t>Traeger_LancetID_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0955395922001153?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Dawe_IJDP_2022.pdf</t>
+  </si>
+  <si>
+    <t>https://www.liebertpub.com/doi/10.1089/AID.2021.0138?url_ver=Z39.88-2003&amp;rfr_id=ori%3Arid%3Acrossref.org&amp;rfr_dat=cr_pub++0pubmed</t>
+  </si>
+  <si>
+    <t>Laher_AIDSRes_2022.pdf</t>
+  </si>
+  <si>
+    <t>https://www.publish.csiro.au/sh/SH22053</t>
+  </si>
+  <si>
+    <t>Traeger_SexHealth_2022.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0955395922000755?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Wilkinson_IJDP_2022.pdf</t>
+  </si>
+  <si>
+    <t>Howell J, **Traeger MW**, Williams B, Layton C, Doyle J, Latham N, Draper B, Bramwell F, Membrey D, McPherson M, Stoové M, Roney J, Thompson A, Hellard M, Pedrana A. The impact of point-of-care hepatitis C testing in needle and syringe exchange programs increases linkage to care and treatment uptake among people who inject drugs: An Australian pilot study. Journal of Viral Hepatitis. 2022;29:275-384. doi:10.1111/jvh.13664</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/jvh.13664</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/epidemiology-and-infection/article/realworld-monitoring-progress-towards-the-elimination-of-hepatitis-c-virus-in-australia-using-sentinel-surveillance-of-primary-care-clinics-an-ecological-study-of-hepatitis-c-virus-antibody-tests-from-2009-to-2019/8D0B1417009BB7EE5BDEBB6C8401A3C7</t>
+  </si>
+  <si>
+    <t>Wilkinson_EpiInfection_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/cid/article/74/10/1804/6410633?login=false</t>
+  </si>
+  <si>
+    <t>Harney_CID_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10461-021-03529-w</t>
+  </si>
+  <si>
+    <t>Howell_JVH_2021.pdf</t>
+  </si>
+  <si>
+    <t>Traeger_AIDSBeh_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(21)00155-7/abstract</t>
+  </si>
+  <si>
+    <t>vanSanten_LancetHIV_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/cid/article/73/7/e2164/5917707</t>
+  </si>
+  <si>
+    <t>Doyle_CID_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ofid/article/8/6/ofab263/6282444?login=false</t>
+  </si>
+  <si>
+    <t>Donovan_OFID_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/jaids/fulltext/2021/08010/brief_report__low_incidence_of_hepatitis_c_among_a.1.aspx</t>
+  </si>
+  <si>
+    <t>Cornelisse_JAIDS_2021.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/aidsonline/fulltext/2021/01010/changes_in_hiv_preexposure_prophylaxis_prescribing.18.aspx</t>
+  </si>
+  <si>
+    <t>Traeger_AIDS_2021.pdf</t>
+  </si>
+  <si>
+    <t>Mwaturura C, **Traeger MW**, Lemoh C, Stoové M, Price B, Coelho A, Mikola M, Ryan K, Wright E. Barriers and Facilitators to Pre-exposure Prophylaxis (PrEP) among African Migrants in High-Income Countries: A Systematic Review. Sexual Health. 2021;18(2):130-139. doi: 10.1071/SH20175</t>
+  </si>
+  <si>
+    <t>Mwaturura_SexualHealth_2021</t>
+  </si>
+  <si>
+    <t>https://www.publish.csiro.au/SH/SH20175</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/stdjournal/fulltext/2020/10000/the_potential_impact_of_a_gel_based_point_of_sex.1.aspx</t>
+  </si>
+  <si>
+    <t>Traeger_STDs_2020.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/stdjournal/fulltext/2020/08000/trends_in_human_immunodeficiency_virus_and.4.aspx</t>
+  </si>
+  <si>
+    <t>Ryan_STDs_2020.pdf</t>
   </si>
 </sst>
 </file>
@@ -1060,31 +1273,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3238FB0-5FA3-6E4B-93CD-C64E98AB6B17}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="4" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="131.5" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" t="s">
         <v>193</v>
-      </c>
-      <c r="B1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1092,15 +1308,15 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="str">
-        <f>CONCATENATE(A2,". ",B2," . **[Link](",C2,"). [PDF](/assets/papers/",D2,").**")</f>
-        <v>1. Allan-Blitz LT, **Traeger MW**, Gitin S, Smith K, Mayer KH, Kahn T. Facilitators and barriers to the rollout of doxycycline post-exposure prophylaxis for sexually transmitted infections in a Boston community health center. Sexually Transmitted Diseases. 2 Jun 2025. doi:10.1097/OLQ.0000000000002190 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <f>CONCATENATE(A2,". ",B2,". **[Link](",C2,"). [PDF](/assets/papers/",D2,").**")</f>
+        <v>1. Allan-Blitz LT, **Traeger MW**, Gitin S, Smith K, Mayer KH, Kahn T. Facilitators and barriers to the rollout of doxycycline post-exposure prophylaxis for sexually transmitted infections in a Boston community health center. Sexually Transmitted Diseases. 2 Jun 2025. doi:10.1097/OLQ.0000000000002190. **[Link]( ). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1108,17 +1324,17 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E43" si="0">CONCATENATE(A3,". ",B3," . **[Link](",C3,"). [PDF](/assets/papers/",D3,").**")</f>
-        <v>2. **Traeger MW**, Leyden WA, Volk JE, Silverberg MJ, Horberg MA, Davis TL, Mayer KH, Krakower DS, Young JG, Jenness SM, Marcus JL. Doxycycline postexposure prophylaxis and sexually transmitted infections among individuals using HIV preexposure prophylaxis. JAMA Internal Medicine. 6 Jan 2025 . **[Link](https://jamanetwork.com/journals/jamainternalmedicine/fullarticle/2828994). [PDF](/assets/papers/Traeger_JAMAIM_2025.pdf).**</v>
+        <f t="shared" ref="E3:E43" si="0">CONCATENATE(A3,". ",B3,". **[Link](",C3,"). [PDF](/assets/papers/",D3,").**")</f>
+        <v>2. **Traeger MW**, Leyden WA, Volk JE, Silverberg MJ, Horberg MA, Davis TL, Mayer KH, Krakower DS, Young JG, Jenness SM, Marcus JL. Doxycycline postexposure prophylaxis and sexually transmitted infections among individuals using HIV preexposure prophylaxis. JAMA Internal Medicine. 6 Jan 2025. **[Link](https://jamanetwork.com/journals/jamainternalmedicine/fullarticle/2828994). [PDF](/assets/papers/Traeger_JAMAIM_2025.pdf).**</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1126,15 +1342,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>3. Mathews R, Shen C, **Traeger MW**, O’Brien HM, Roder C, Hellard ME, Doyle JS. Enhancing hepatitis C virus testing, linkage to care and treatment commencement in hospitals a systematic review and meta-analysis. Open Forum Infectious Diseases. Accepted 3 Feb 2025 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>3. Mathews R, Shen C, **Traeger MW**, O’Brien HM, Roder C, Hellard ME, Doyle JS. Enhancing hepatitis C virus testing, linkage to care and treatment commencement in hospitals a systematic review and meta-analysis. Open Forum Infectious Diseases. Accepted 3 Feb 2025. **[Link](https://academic.oup.com/ofid/article/12/2/ofaf056/7998417?login=false). [PDF](/assets/papers/Matthews_OFID_2025.pdf).**</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1145,12 +1363,14 @@
         <v>73</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>4. Shen C, Dawe J, **Traeger MW**, Sacks-Davis R, Pedrana AE, Doyle JS, Hellard ME, Stoové M. Financial incentives to increase engagement across the hepatitis C care cascade among people at risk of or diagnosed with hepatitis C: A systematic review. International Journal of Drug Policy. 2024;133:104562. doi:10.1016/j.drugpo.2024.104562 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>4. Shen C, Dawe J, **Traeger MW**, Sacks-Davis R, Pedrana AE, Doyle JS, Hellard ME, Stoové M. Financial incentives to increase engagement across the hepatitis C care cascade among people at risk of or diagnosed with hepatitis C: A systematic review. International Journal of Drug Policy. 2024;133:104562. doi:10.1016/j.drugpo.2024.104562. **[Link](https://www.sciencedirect.com/science/article/pii/S0955395924002469?via%3Dihub). [PDF](/assets/papers/Shen_IJDP_2024.pdf).**</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1161,12 +1381,12 @@
         <v>74</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>5. Medland NA, McManus H, Bavinton BR, Fraser D, **Traeger MW**, Grulich AE, Stoové M, McGregor S, King JM, Heath-Paynter D, Guy RJ. HIV incidence in people receiving government-subsidised pre-exposure prophylaxis in Australia: a whole-of-population retrospective cohort study. The Lancet HIV. Online first 27 Sep 2024. doi:10.1016/S2352-3018(24)00213-3 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>5. Medland NA, McManus H, Bavinton BR, Fraser D, **Traeger MW**, Grulich AE, Stoové M, McGregor S, King JM, Heath-Paynter D, Guy RJ. HIV incidence in people receiving government-subsidised pre-exposure prophylaxis in Australia: a whole-of-population retrospective cohort study. The Lancet HIV. Online first 27 Sep 2024. doi:10.1016/S2352-3018(24)00213-3. **[Link](https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(24)00213-3/abstract). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1177,12 +1397,14 @@
         <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>209</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>6. **Traeger MW**, Guy R, Asselin J, et al. Syphilis testing, incidence and reinfection among gay and bisexual men in Australia over a decade spanning HIV PrEP implementation: an analysis of surveillance data from 2012-2022. The Lancet Regional Health – Western Pacific.2024;51:101175 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>6. **Traeger MW**, Guy R, Asselin J, et al. Syphilis testing, incidence and reinfection among gay and bisexual men in Australia over a decade spanning HIV PrEP implementation: an analysis of surveillance data from 2012-2022. The Lancet Regional Health – Western Pacific.2024;51:101175. **[Link](https://www.thelancet.com/journals/lanwpc/article/PIIS2666-6065(24)00169-X/fulltext). [PDF](/assets/papers/Traeger_LancetRHWP_2024.pdf).**</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1193,12 +1415,14 @@
         <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>7. Harney BL, Sacks-Davis R, **Traeger MW**, van Santen DK, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews G, Donovan B, Guy R, Hellard ME, Doyle JS. Annual hepatitis C testing and positive tests among gay and bisexual men in Australia from 2016 to 2022: a serial cross-sectional analysis of sentinel surveillance data. Sexually transmitted infections. 2024;100:295-301. doi:10.1136/sextrans-2024-056175 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>7. Harney BL, Sacks-Davis R, **Traeger MW**, van Santen DK, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews G, Donovan B, Guy R, Hellard ME, Doyle JS. Annual hepatitis C testing and positive tests among gay and bisexual men in Australia from 2016 to 2022: a serial cross-sectional analysis of sentinel surveillance data. Sexually transmitted infections. 2024;100:295-301. doi:10.1136/sextrans-2024-056175. **[Link](https://sti.bmj.com/content/100/5/295.long). [PDF](/assets/papers/Harney_STI_2024.pdf).**</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1206,15 +1430,17 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>214</v>
+      </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>8. **Traeger MW**, Krakower DS, Mayer KH, Jenness SM, Marcus JL. Use of doxycycline and other antibiotics as bacterial sexually transmitted infection prophylaxis in a U.S. sample of primarily gay and bisexual men. Sexually Transmitted Diseases. Online 8 Aug 2024. doi:10.1097/OLQ.0000000000002061 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>8. **Traeger MW**, Krakower DS, Mayer KH, Jenness SM, Marcus JL. Use of doxycycline and other antibiotics as bacterial sexually transmitted infection prophylaxis in a U.S. sample of primarily gay and bisexual men. Sexually Transmitted Diseases. Online 8 Aug 2024. doi:10.1097/OLQ.0000000000002061. **[Link](https://journals.lww.com/stdjournal/fulltext/2024/12000/use_of_doxycycline_and_other_antibiotics_as.1.aspx). [PDF](/assets/papers/Traeger_STDs_2024.pdf).**</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1225,12 +1451,14 @@
         <v>77</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>216</v>
+      </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>9. Hayes MJ, Beavon E, **Traeger MW**, Dillon JF, Radley A, Nielsen S, Byrne CJ, Richmond J, Higgs P, Hellard M, Doyle JS. Viral hepatitis testing and treatment in community pharmacies: a systematic review and meta-analysis. eClinial Medicine. 2024 Feb 27;69:102489. doi:10.1016/j.eclinm.2024.102489 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>9. Hayes MJ, Beavon E, **Traeger MW**, Dillon JF, Radley A, Nielsen S, Byrne CJ, Richmond J, Higgs P, Hellard M, Doyle JS. Viral hepatitis testing and treatment in community pharmacies: a systematic review and meta-analysis. eClinial Medicine. 2024 Feb 27;69:102489. doi:10.1016/j.eclinm.2024.102489. **[Link](https://linkinghub.elsevier.com/retrieve/pii/S2589-5370(24)00068-3). [PDF](/assets/papers/Hayes_cClinMed_2024.pdf).**</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,15 +1466,17 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>217</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>10. Harney BL, Sacks-Davis R, Paul Agius, van Santen DK, **Traeger MW**, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews GV, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. Risk of primary incident hepatitis C infection following bacterial sexually transmissible infections among gay and bisexual men in Australia from 2016 to 2020. Open Forum Infectious Diseases. Online 19 Feb 2024 doi:10.1093/ofid/ofae099 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>10. Harney BL, Sacks-Davis R, Paul Agius, van Santen DK, **Traeger MW**, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews GV, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. Risk of primary incident hepatitis C infection following bacterial sexually transmissible infections among gay and bisexual men in Australia from 2016 to 2020. Open Forum Infectious Diseases. Online 19 Feb 2024 doi:10.1093/ofid/ofae099. **[Link](https://academic.oup.com/ofid/article/11/4/ofae099/7610685). [PDF](/assets/papers/Harney_OFID_2024.pdf).**</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,12 +1487,14 @@
         <v>78</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>11. Harney BL, Sacks-Davis R, van Santen DK, **Traeger MW**, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews GV, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. Hepatitis C virus reinfection incidence among gay and bisexual men with HIV in Australia from 2016 to 2020. Liver International. Online 21 Jan 2024. doi:10.1111/liv.15841 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>11. Harney BL, Sacks-Davis R, van Santen DK, **Traeger MW**, Wilkinson AL, Asselin J, Fairley CK, Roth N, Bloch M, Matthews GV, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. Hepatitis C virus reinfection incidence among gay and bisexual men with HIV in Australia from 2016 to 2020. Liver International. Online 21 Jan 2024. doi:10.1111/liv.15841. **[Link](https://onlinelibrary.wiley.com/doi/10.1111/liv.15841). [PDF](/assets/papers/Harney_LiverInt_2024.pdf).**</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1273,12 +1505,14 @@
         <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>221</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>12. Nevendorrf L, Pedrana A, Bourne A, Traeger M, Sindunata E, Reswana WA, Alharbi RM, Stoové M. Characterizing socioecological markers of differentiated HIV risk among men who have sex with men in Indonesia. AIDS and Behavior. Online 25 Jan 2024. doi:10.1007/s10461-023-04253-3 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>12. Nevendorrf L, Pedrana A, Bourne A, Traeger M, Sindunata E, Reswana WA, Alharbi RM, Stoové M. Characterizing socioecological markers of differentiated HIV risk among men who have sex with men in Indonesia. AIDS and Behavior. Online 25 Jan 2024. doi:10.1007/s10461-023-04253-3. **[Link](https://link.springer.com/article/10.1007/s10461-023-04253-3). [PDF](/assets/papers/Nevendorrf_AIDSBeh_2024.pdf).**</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,12 +1523,14 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>223</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>13. Chan C, Holt M, Broady TR, Traeger M, Mao L, Grulich AE, Prestage G, MacGibbon J, Rule J, Bavinton BR. Trends in testing and self-reported diagnoses of sexually transmitted infections in gay and bisexual men in Australia, 2017-2021: analysis of national behavioural surveillance surveys. Sexually Transmitted Diseases. Online 9 Oct 2023. doi:10.1097/OLQ.0000000000001870 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>13. Chan C, Holt M, Broady TR, Traeger M, Mao L, Grulich AE, Prestage G, MacGibbon J, Rule J, Bavinton BR. Trends in testing and self-reported diagnoses of sexually transmitted infections in gay and bisexual men in Australia, 2017-2021: analysis of national behavioural surveillance surveys. Sexually Transmitted Diseases. Online 9 Oct 2023. doi:10.1097/OLQ.0000000000001870. **[Link](https://journals.lww.com/stdjournal/fulltext/2023/12000/trends_in_testing_and_self_reported_diagnoses_of.3.aspx). [PDF](/assets/papers/Chan_STDs_2023.pdf).**</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1305,12 +1541,14 @@
         <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>14. Cornelisse VJ, Murphy D, Lee SJ, Stoove M, **Traeger MW**, Wright EJ. Physical and mental health of long-term users of HIV pre-exposure prophylaxis (PrEP) in Australia: The X-PLORE Cohort. AIDS. Online 26 Oct 2023. doi:10.1097/QAD.0000000000003678 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>14. Cornelisse VJ, Murphy D, Lee SJ, Stoove M, **Traeger MW**, Wright EJ. Physical and mental health of long-term users of HIV pre-exposure prophylaxis (PrEP) in Australia: The X-PLORE Cohort. AIDS. Online 26 Oct 2023. doi:10.1097/QAD.0000000000003678. **[Link](https://journals.lww.com/aidsonline/abstract/2024/03010/physical_and_mental_health_of_long_term_users_of.10.aspx). [PDF](/assets/papers/Cornelisse_AIDS_2023.pdf).**</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,15 +1556,17 @@
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>229</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>15. Munari SC*, **Traeger MW***, Menon V, Latham NH, Manoharan L, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Conway B, Klein M, Bruneau J, Stoové MA, Hellard ME, Doyle JS. Determining reinfection rates by hepatitis C testing interval among key populations: a systematic review and meta-analysis. Online 10 Oct 2023. doi:10.1111/liv.15705 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>15. Munari SC (co-first), **Traeger MW (co-first)**, Menon V, Latham NH, Manoharan L, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Conway B, Klein M, Bruneau J, Stoové MA, Hellard ME, Doyle JS. Determining reinfection rates by hepatitis C testing interval among key populations: a systematic review and meta-analysis. Online 10 Oct 2023. doi:10.1111/liv.15705. **[Link](https://onlinelibrary.wiley.com/doi/10.1111/liv.15705). [PDF](/assets/papers/Munari_LiverInt_2023.pdf).**</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1334,15 +1574,17 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>230</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>231</v>
+      </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>16. Mayer KH, **Traeger MW**, Marcus JL. Doxycycline Postexposure Prophylaxis and Sexually Transmitted Infections. Journal of the American Medical Association. Online 22 Sep 2023. doi:10.1001/jama.2023.16416 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>16. Mayer KH, **Traeger MW**, Marcus JL. Doxycycline Postexposure Prophylaxis and Sexually Transmitted Infections. Journal of the American Medical Association. Online 22 Sep 2023. doi:10.1001/jama.2023.16416. **[Link](https://jamanetwork.com/journals/jama/fullarticle/2810020). [PDF](/assets/papers/Mayer_JAMA_2023.pdf).**</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1350,15 +1592,17 @@
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>17. **Traeger MW**, Mayer KH, Krakower DS, Gitin S, Jenness SM, Marcus JL. Potential impact of doxycycline post-exposure prophylaxis prescribing strategies on incidence of bacterial sexually transmitted infections. Clinical Infectious Diseases. Online 18 Aug 2023. doi:10.1093/cid/ciad488 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>17. **Traeger MW**, Mayer KH, Krakower DS, Gitin S, Jenness SM, Marcus JL. Potential impact of doxycycline post-exposure prophylaxis prescribing strategies on incidence of bacterial sexually transmitted infections. Clinical Infectious Diseases. Online 18 Aug 2023. doi:10.1093/cid/ciad488. **[Link](https://academic.oup.com/cid/advance-article/doi/10.1093/cid/ciad488/7245976). [PDF](/assets/papers/Traeger_CID_2023.pdf).**</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1366,15 +1610,17 @@
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>234</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>18. **Traeger MW**, Krakower DS, Mayer KH, Marcus JL. Prioritising the values of potential users to promote uptake of HIV pre-exposure prophylaxis. Lancet HIV. Online 10 Aug 2023. doi:10.1016/S2352-3018(23)00171-6 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>18. **Traeger MW**, Krakower DS, Mayer KH, Marcus JL. Prioritising the values of potential users to promote uptake of HIV pre-exposure prophylaxis. Lancet HIV. Online 10 Aug 2023. doi:10.1016/S2352-3018(23)00171-6. **[Link](https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(23)00171-6/abstract). [PDF](/assets/papers/Traeger_LancetHIV_2023.pdf).**</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,15 +1628,17 @@
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>236</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>19. **Traeger MW**, Harney BL, Sacks-Davis R, van Santen DK, Cornelisse V, Wright EJ, Hellard ME, Doyle JS, Stoové MA. Incidence and prevalence of hepatitis C virus among HIV-negative gay and bisexual men using HIV pre-exposure prophylaxis (PrEP): a systematic review and meta-analysis. Open Forum Infectious Diseases. 01 August 2023. doi:10.1093/ofid/ofad401 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>19. **Traeger MW**, Harney BL, Sacks-Davis R, van Santen DK, Cornelisse V, Wright EJ, Hellard ME, Doyle JS, Stoové MA. Incidence and prevalence of hepatitis C virus among HIV-negative gay and bisexual men using HIV pre-exposure prophylaxis (PrEP): a systematic review and meta-analysis. Open Forum Infectious Diseases. 01 August 2023. doi:10.1093/ofid/ofad401. **[Link](https://academic.oup.com/ofid/article/10/8/ofad401/7234598). [PDF](/assets/papers/Traeger_OFID_2023.pdf).**</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1398,15 +1646,17 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>238</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>20. Manoharan L, Latham NH, Munari SC, **Traeger MW**, Menon V, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Matthews GV, Stoové M, Hellard M, Doyle JS. Immediate treatment for recent hepatitis C infection in people with high-risk behaviours: a systematic review and meta-analysis. Hepatology Communications. 7(4):e0082, April 2023. doi:10.1097/HC9.0000000000000082 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>20. Manoharan L, Latham NH, Munari SC, **Traeger MW**, Menon V, Luhmann N, Baggaley R, MacDonald V, Verster A, Siegfried N, Matthews GV, Stoové M, Hellard M, Doyle JS. Immediate treatment for recent hepatitis C infection in people with high-risk behaviours: a systematic review and meta-analysis. Hepatology Communications. 7(4):e0082, April 2023. doi:10.1097/HC9.0000000000000082. **[Link](https://journals.lww.com/hepcomm/fulltext/2023/04010/immediate_treatment_for_recent_hepatitis_c.2.aspx). [PDF](/assets/papers/Manoharan_HepComm_2023.pdf).**</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1414,15 +1664,17 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>21. **Traeger MW**, Doyle JS,  van Santen DK, Sacks-Davis R, Asselin J, El-Hayek C, Pedrana A, Wilkinson AL, Howell J, Membrey D, Didlick J, Donovan B, Guy R, Hellard ME, Stoové MA. Impact of COVID-19 lockdown restrictions on hepatitis C testing in Australian primary care and community health services providing care for people who inject drugs. Journal of Viral Hepatitis. Online 20 June 2022. doi:10.1111/jvh.13723 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>21. **Traeger MW**, Doyle JS,  van Santen DK, Sacks-Davis R, Asselin J, El-Hayek C, Pedrana A, Wilkinson AL, Howell J, Membrey D, Didlick J, Donovan B, Guy R, Hellard ME, Stoové MA. Impact of COVID-19 lockdown restrictions on hepatitis C testing in Australian primary care and community health services providing care for people who inject drugs. Journal of Viral Hepatitis. Online 20 June 2022. doi:10.1111/jvh.13723. **[Link](https://onlinelibrary.wiley.com/doi/10.1111/jvh.13723). [PDF](/assets/papers/Traeger_JVHep_2023.pdf).**</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1430,15 +1682,17 @@
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>242</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>22. **Traeger MW**, Guy R Asselin J, Patel P, Carter A, Wright E, Grulich A, McManus H, Fairley CK, Chow EPF, McNulty A, Finlayson R, Bell C, Owen L, Marshall L, Russell D, O’Donnell D, Donovan B, Hellard ME, Stoové MA. Real-world trends in incidence of bacterial sexually transmissible infections among gay and bisexual men using HIV pre-exposure prophylaxis following nation-wide pre-exposure prophylaxis implementation in Australia: an analysis of sentinel surveillance data. The Lancet Infectious Diseases. Online 25 May 2022. doi:10.1016/S1473-3099(22)00175X . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>22. **Traeger MW**, Guy R Asselin J, Patel P, Carter A, Wright E, Grulich A, McManus H, Fairley CK, Chow EPF, McNulty A, Finlayson R, Bell C, Owen L, Marshall L, Russell D, O’Donnell D, Donovan B, Hellard ME, Stoové MA. Real-world trends in incidence of bacterial sexually transmissible infections among gay and bisexual men using HIV pre-exposure prophylaxis following nation-wide pre-exposure prophylaxis implementation in Australia: an analysis of sentinel surveillance data. The Lancet Infectious Diseases. Online 25 May 2022. doi:10.1016/S1473-3099(22)00175X. **[Link](https://linkinghub.elsevier.com/retrieve/pii/S1473-3099(22)00175-X). [PDF](/assets/papers/Traeger_LancetID_2023.pdf).**</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1446,15 +1700,17 @@
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>244</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>23. Dawe J, Wilkinson A, Asselin J, Pedrana A, **Traeger MW**, Thomas A, Curtis M, Howell J, Doyle J, Hellard M, Stoové M. Hepatitis C antibody testing among opioid agonist therapy recipients, Victoria, Australia, 2012 to 2020. International Journal of Drug Policy. 2022 Jun;104:103696. doi:10.1016/j.drugpo.2022.103696 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>23. Dawe J, Wilkinson A, Asselin J, Pedrana A, **Traeger MW**, Thomas A, Curtis M, Howell J, Doyle J, Hellard M, Stoové M. Hepatitis C antibody testing among opioid agonist therapy recipients, Victoria, Australia, 2012 to 2020. International Journal of Drug Policy. 2022 Jun;104:103696. doi:10.1016/j.drugpo.2022.103696. **[Link](https://www.sciencedirect.com/science/article/abs/pii/S0955395922001153?via%3Dihub). [PDF](/assets/papers/Dawe_IJDP_2022.pdf).**</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1462,15 +1718,17 @@
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>246</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>24. Laher F, Richardson SI, Smith P, Sullivan PS, Abrahams AG, Asowata OE, Bitangumutwenzi P, Dabee S, Dollah A, Fernandez N, Langat RK, Bose DL, Likhitwonnawut U, Mullick R, Resop RS, Sutar J, Thompson-Hall AN, **Traeger MW**, Tuyishime M, Wambui J, Bekker L, Kaleebu P, McCormack S, O’Connor DH, Warren M, Torri T, Thyagarajan B. HIV prevention in a time of COVID-19: A report from the HIVR4P // Virtual conference 2021. AIDS Research and Human Retroviruses. 2022 May;38(5):350-358. doi: 10.1089/AID.2021.0138 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>24. Laher F, Richardson SI, Smith P, Sullivan PS, Abrahams AG, Asowata OE, Bitangumutwenzi P, Dabee S, Dollah A, Fernandez N, Langat RK, Bose DL, Likhitwonnawut U, Mullick R, Resop RS, Sutar J, Thompson-Hall AN, **Traeger MW**, Tuyishime M, Wambui J, Bekker L, Kaleebu P, McCormack S, O’Connor DH, Warren M, Torri T, Thyagarajan B. HIV prevention in a time of COVID-19: A report from the HIVR4P // Virtual conference 2021. AIDS Research and Human Retroviruses. 2022 May;38(5):350-358. doi: 10.1089/AID.2021.0138. **[Link](https://www.liebertpub.com/doi/10.1089/AID.2021.0138?url_ver=Z39.88-2003&amp;rfr_id=ori%3Arid%3Acrossref.org&amp;rfr_dat=cr_pub++0pubmed). [PDF](/assets/papers/Laher_AIDSRes_2022.pdf).**</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1478,15 +1736,17 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>248</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>25. **Traeger MW**, Stoové MA. Why risk matter for STI control: who are those at greatest risk and how are they identified? Sexual Health. Accepted 26 Apr 2022 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>25. **Traeger MW**, Stoové MA. Why risk matter for STI control: who are those at greatest risk and how are they identified? Sexual Health. Accepted 26 Apr 2022. **[Link](https://www.publish.csiro.au/sh/SH22053). [PDF](/assets/papers/Traeger_SexHealth_2022.pdf).**</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,15 +1754,17 @@
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>250</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>26. Wilkinson AL, van Santen DK, **Traeger MW**, Sacks-Davis R, Asselin J, Scott N, Harney B, Doyle JS, El-Hayek C, Howell J, Bramwell F, McManus H, Donovan B, Guy R, Stoové M, Hellard M, Pedrana A. Hepatitis C incidence among patients attending primary care health services that specialise in the care of people who inject drugs, Victoria, Australia, 2009 to 2020. International Journal of Drug Policy. 2022Mar 25;103:103655. doi:10.1016/j.drugpo.2022.103655 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>26. Wilkinson AL, van Santen DK, **Traeger MW**, Sacks-Davis R, Asselin J, Scott N, Harney B, Doyle JS, El-Hayek C, Howell J, Bramwell F, McManus H, Donovan B, Guy R, Stoové M, Hellard M, Pedrana A. Hepatitis C incidence among patients attending primary care health services that specialise in the care of people who inject drugs, Victoria, Australia, 2009 to 2020. International Journal of Drug Policy. 2022Mar 25;103:103655. doi:10.1016/j.drugpo.2022.103655. **[Link](https://www.sciencedirect.com/science/article/pii/S0955395922000755?via%3Dihub). [PDF](/assets/papers/Wilkinson_IJDP_2022.pdf).**</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1510,15 +1772,17 @@
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>253</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>27. Howell J, **Traeger MW**, Williams B, Layton C, Doyle J, Latham N, Draper B, Bramwell F, Membrey D, McPherson M, Stoové M, Roney J, Thompson A, Hellard M, Pedrana A. Point-of-care hepatitis C testing in needle and syringe exchange programs increases linkage to care and treatment uptake among people who inject drugs: An Australian pilot study. Journal of Viral Hepatitis. 2022;29:275-384. doi:10.1111/jvh.13664 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>27. Howell J, **Traeger MW**, Williams B, Layton C, Doyle J, Latham N, Draper B, Bramwell F, Membrey D, McPherson M, Stoové M, Roney J, Thompson A, Hellard M, Pedrana A. The impact of point-of-care hepatitis C testing in needle and syringe exchange programs increases linkage to care and treatment uptake among people who inject drugs: An Australian pilot study. Journal of Viral Hepatitis. 2022;29:275-384. doi:10.1111/jvh.13664. **[Link](https://onlinelibrary.wiley.com/doi/10.1111/jvh.13664). [PDF](/assets/papers/Howell_JVH_2021.pdf).**</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1526,15 +1790,17 @@
         <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>254</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>28. Wilkinson AL, Pedrana A, **Traeger MW**, Asselin J, El-Hayek C, Nguyen L, Polkinghorne V, Doyle JS, Thompson AJ, Howell J, Scott N, Dimech W, Guy R, Stoové M, Hellard M. Real world monitoring progress towards the elimination of hepatitis C virus in Australia using sentinel surveillance of primary care clinics: an ecological study of hepatitis C virus antibody tests from 2009 to 2019. Epidemiology and infection. 2021 Dec 6;150:e7. doi:10.1017/S0950268821002624 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>28. Wilkinson AL, Pedrana A, **Traeger MW**, Asselin J, El-Hayek C, Nguyen L, Polkinghorne V, Doyle JS, Thompson AJ, Howell J, Scott N, Dimech W, Guy R, Stoové M, Hellard M. Real world monitoring progress towards the elimination of hepatitis C virus in Australia using sentinel surveillance of primary care clinics: an ecological study of hepatitis C virus antibody tests from 2009 to 2019. Epidemiology and infection. 2021 Dec 6;150:e7. doi:10.1017/S0950268821002624. **[Link](https://www.cambridge.org/core/journals/epidemiology-and-infection/article/realworld-monitoring-progress-towards-the-elimination-of-hepatitis-c-virus-in-australia-using-sentinel-surveillance-of-primary-care-clinics-an-ecological-study-of-hepatitis-c-virus-antibody-tests-from-2009-to-2019/8D0B1417009BB7EE5BDEBB6C8401A3C7). [PDF](/assets/papers/Wilkinson_EpiInfection_2021.pdf).**</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1542,15 +1808,17 @@
         <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>256</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>257</v>
+      </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>29. Harney BL, Sacks-Davis R, van Santen DK, **Traeger MW**, Wilkinson A, Asselin J, El-Hayek C, Fairley CK, Roth N, Bloch M, Matthews G, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. The incidence of hepatitis C among gay, bisexual and other men who have sex with men before and after the availability of direct acting antivirals in Australia, 2009-2019. Clinical Infectious Diseases. Online 25 October 2021. doi:10.1093/cid/ciab720 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>29. Harney BL, Sacks-Davis R, van Santen DK, **Traeger MW**, Wilkinson A, Asselin J, El-Hayek C, Fairley CK, Roth N, Bloch M, Matthews G, Donovan B, Guy R, Stoové M, Hellard ME, Doyle JS. The incidence of hepatitis C among gay, bisexual and other men who have sex with men before and after the availability of direct acting antivirals in Australia, 2009-2019. Clinical Infectious Diseases. Online 25 October 2021. doi:10.1093/cid/ciab720. **[Link](https://academic.oup.com/cid/article/74/10/1804/6410633?login=false). [PDF](/assets/papers/Harney_CID_2021.pdf).**</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1558,15 +1826,17 @@
         <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>258</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>30. **Traeger MW**, Murphy D, Ryan K, Asselin J, Cornelisse V, Hellard M, Wright E, Stoové M. Latent class analysis of sexual behaviors and attitudes to sexually transmitted infections among gay and bisexual men using PrEP. AIDS and Behavior. (2021). doi:10.1007/s10461-021-03529-w . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>30. **Traeger MW**, Murphy D, Ryan K, Asselin J, Cornelisse V, Hellard M, Wright E, Stoové M. Latent class analysis of sexual behaviors and attitudes to sexually transmitted infections among gay and bisexual men using PrEP. AIDS and Behavior. (2021). doi:10.1007/s10461-021-03529-w. **[Link](https://link.springer.com/article/10.1007/s10461-021-03529-w). [PDF](/assets/papers/Traeger_AIDSBeh_2021.pdf).**</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1574,15 +1844,17 @@
         <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>261</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>31. Van Santen DK, Asselin J, Haber NA, **Traeger MW**, Callander D, Donovan B, El-Hayek C, McMahon JH, Petoumenos K, McManus H, Hoy J, Hellard M, Guy R, Stoové MA. Improvements in transition times through the HIV cascade of care among gay and bisexual men with a new HIV diagnosis in New South Wales and Victoria, Australia: the longitudinal HIV cascade (2012-2019). The Lancet HIV. 2021 Oct;8(10):e623-e632. doi:10.1016/S2352-3018(21)00155-7 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>31. Van Santen DK, Asselin J, Haber NA, **Traeger MW**, Callander D, Donovan B, El-Hayek C, McMahon JH, Petoumenos K, McManus H, Hoy J, Hellard M, Guy R, Stoové MA. Improvements in transition times through the HIV cascade of care among gay and bisexual men with a new HIV diagnosis in New South Wales and Victoria, Australia: the longitudinal HIV cascade (2012-2019). The Lancet HIV. 2021 Oct;8(10):e623-e632. doi:10.1016/S2352-3018(21)00155-7. **[Link](https://www.thelancet.com/journals/lanhiv/article/PIIS2352-3018(21)00155-7/abstract). [PDF](/assets/papers/vanSanten_LancetHIV_2021.pdf).**</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1591,15 +1863,17 @@
         <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>263</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>32. Doyle JS, van Santen DK, Iser d, Sasadeusz J, O’Reilly M, Harney B, **Traeger MW**, Roney J, Cutts JC, Bowring AL, Winter R, Medland N, Fairley CK, Moore R, Tee BK, Asselin J, El-Hayek C, Hoy JF, Matthews CV, Prins M, Stoové MA, Hellard ME. Mirco-elimination of Hepatitis C among People with HIV Coinfection: Declining Incidence and Prevalence Accompanying a Multi-center Treatment Scale-up Trial. Clinical Infectious Diseases. 2021 Oct 5;73(7):e2164-e2172. doi:10.1093/cid/cia1500 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>32. Doyle JS, van Santen DK, Iser d, Sasadeusz J, O’Reilly M, Harney B, **Traeger MW**, Roney J, Cutts JC, Bowring AL, Winter R, Medland N, Fairley CK, Moore R, Tee BK, Asselin J, El-Hayek C, Hoy JF, Matthews CV, Prins M, Stoové MA, Hellard ME. Mirco-elimination of Hepatitis C among People with HIV Coinfection: Declining Incidence and Prevalence Accompanying a Multi-center Treatment Scale-up Trial. Clinical Infectious Diseases. 2021 Oct 5;73(7):e2164-e2172. doi:10.1093/cid/cia1500. **[Link](https://academic.oup.com/cid/article/73/7/e2164/5917707). [PDF](/assets/papers/Doyle_CID_2021.pdf).**</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1607,15 +1881,17 @@
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>265</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>33. Donovan LC, Fairley CK, Aung ET, **Traeger MW**, Wright EJ, Stoové MA, Chow EPF. The presence or absence of symptoms among cases of urethral gonorrhoea occurring in a cohort of men taking HIV pre-exposure prophylaxis in the PrEPX Study. Open Forum Infectious Diseases. 2021;8(6):ofab263. doi: 10.1093/ofid/ofab263 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>33. Donovan LC, Fairley CK, Aung ET, **Traeger MW**, Wright EJ, Stoové MA, Chow EPF. The presence or absence of symptoms among cases of urethral gonorrhoea occurring in a cohort of men taking HIV pre-exposure prophylaxis in the PrEPX Study. Open Forum Infectious Diseases. 2021;8(6):ofab263. doi: 10.1093/ofid/ofab263. **[Link](https://academic.oup.com/ofid/article/8/6/ofab263/6282444?login=false). [PDF](/assets/papers/Donovan_OFID_2021.pdf).**</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1623,15 +1899,17 @@
         <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D35" s="3"/>
+        <v>267</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>268</v>
+      </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>34. Cornelisse VJ, **Traeger MW**, Wright EJ, Murphy D, Stoové M, Hellard M, Sacks-Davis R, Asselin J, Fairley CK, Doyle J, Sasadeusz J. Low incidence of hepatitis C among a cohort of HIV-negative gay and bisexual men using HIV pre-exposure prophylaxis (PrEP) in Melbourne, Australia, and the contribution of sexual transmission. Journal of Acquired Immune Deficiency Syndromes. 2021;87(4):1011-1015. doi: 10.1097/QAI.0000000000002685 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>34. Cornelisse VJ, **Traeger MW**, Wright EJ, Murphy D, Stoové M, Hellard M, Sacks-Davis R, Asselin J, Fairley CK, Doyle J, Sasadeusz J. Low incidence of hepatitis C among a cohort of HIV-negative gay and bisexual men using HIV pre-exposure prophylaxis (PrEP) in Melbourne, Australia, and the contribution of sexual transmission. Journal of Acquired Immune Deficiency Syndromes. 2021;87(4):1011-1015. doi: 10.1097/QAI.0000000000002685. **[Link](https://journals.lww.com/jaids/fulltext/2021/08010/brief_report__low_incidence_of_hepatitis_c_among_a.1.aspx). [PDF](/assets/papers/Cornelisse_JAIDS_2021.pdf).**</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1639,15 +1917,17 @@
         <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>269</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>270</v>
+      </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>35. **Traeger MW**, Patel P, Guy R, Hellard M, Stoové M. Changes in HIV pre-exposure prophylaxis prescribing in Australian clinical services following COVID-10 restrictions. AIDS. 2021;35(1):155-157. doi:10.1097/QAD.0000000000002703 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>35. **Traeger MW**, Patel P, Guy R, Hellard M, Stoové M. Changes in HIV pre-exposure prophylaxis prescribing in Australian clinical services following COVID-10 restrictions. AIDS. 2021;35(1):155-157. doi:10.1097/QAD.0000000000002703. **[Link](https://journals.lww.com/aidsonline/fulltext/2021/01010/changes_in_hiv_preexposure_prophylaxis_prescribing.18.aspx). [PDF](/assets/papers/Traeger_AIDS_2021.pdf).**</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1655,15 +1935,17 @@
         <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>100</v>
+        <v>271</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>273</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>36. Mwaturura C, **Traeger MW**, Lemoh C, Stoové M, Price B, Coelho A, Mikola M, Ryan K, Wright E. Acceptability, Willingness to Use, Barriers and Facilitators to Pre-exposure Prophylaxis (PrEP) among African Migrants in High-Income Countries: A Systematic Review. Sexual Health. 2021;18(2):130-139. doi: 10.1071/SH20175 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>36. Mwaturura C, **Traeger MW**, Lemoh C, Stoové M, Price B, Coelho A, Mikola M, Ryan K, Wright E. Barriers and Facilitators to Pre-exposure Prophylaxis (PrEP) among African Migrants in High-Income Countries: A Systematic Review. Sexual Health. 2021;18(2):130-139. doi: 10.1071/SH20175. **[Link](https://www.publish.csiro.au/SH/SH20175). [PDF](/assets/papers/Mwaturura_SexualHealth_2021).**</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1671,15 +1953,17 @@
         <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D38" s="3"/>
+        <v>274</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>275</v>
+      </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>37. **Traeger MW**, Tidhar T, Holt M, Williams C, Wright E, Stoové M, Scott N, Hellard M. The Potential Impact of a Gel-based Point-of-sex Intervention in Reducing Gonorrhoea Incidence among Gay and Bisexual Men: a Modelling Study. Sexually Transmitted Diseases. 2020; 47(10): 649-657. doi:10.1097/OLQ.0000000000001239 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>37. **Traeger MW**, Tidhar T, Holt M, Williams C, Wright E, Stoové M, Scott N, Hellard M. The Potential Impact of a Gel-based Point-of-sex Intervention in Reducing Gonorrhoea Incidence among Gay and Bisexual Men: a Modelling Study. Sexually Transmitted Diseases. 2020; 47(10): 649-657. doi:10.1097/OLQ.0000000000001239. **[Link](https://journals.lww.com/stdjournal/fulltext/2020/10000/the_potential_impact_of_a_gel_based_point_of_sex.1.aspx). [PDF](/assets/papers/Traeger_STDs_2020.pdf).**</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1690,12 +1974,14 @@
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>276</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>38. Ryan KE, Asselin J, Fairley CK, Armishaw J, Lal L, Nguyen L, Murphy D, Traeger M, Hellard M, Hoy J, Stoové M, Wright E. Trends in HIV and STI testing among gay bisexual and other men who have sex with men following rapid scale-up of PrEP in Victoria, Australia. Sexually Transmitted Diseases. 2020; 47(8): 516-24. doi: 10.1097/OLQ.0000000000001187 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>38. Ryan KE, Asselin J, Fairley CK, Armishaw J, Lal L, Nguyen L, Murphy D, Traeger M, Hellard M, Hoy J, Stoové M, Wright E. Trends in HIV and STI testing among gay bisexual and other men who have sex with men following rapid scale-up of PrEP in Victoria, Australia. Sexually Transmitted Diseases. 2020; 47(8): 516-24. doi: 10.1097/OLQ.0000000000001187. **[Link](https://journals.lww.com/stdjournal/fulltext/2020/08000/trends_in_human_immunodeficiency_virus_and.4.aspx). [PDF](/assets/papers/Ryan_STDs_2020.pdf).**</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1703,15 +1989,15 @@
         <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>39. **Traeger MW**, Pedrana A, van Santen DK, Doyle JS, Howell J, Thompson A, El-Hayek C, Asselin J, Nguyen L, Polkinghorne V, Membrey D, Bramwell F, Carter A, Guy R, Stoové M, Hellard M. The Impact of Universal Access to Direct-Acting Antiviral Therapy on the Hepatitis C Cascade of Care among Individuals attending Primary and Community Health Services. PLoS ONE. 2020; 15(6):e0235445. doi:10.1371/journal.pone.0235445 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>39. **Traeger MW**, Pedrana A, van Santen DK, Doyle JS, Howell J, Thompson A, El-Hayek C, Asselin J, Nguyen L, Polkinghorne V, Membrey D, Bramwell F, Carter A, Guy R, Stoové M, Hellard M. The Impact of Universal Access to Direct-Acting Antiviral Therapy on the Hepatitis C Cascade of Care among Individuals attending Primary and Community Health Services. PLoS ONE. 2020; 15(6):e0235445. doi:10.1371/journal.pone.0235445. **[Link]( ). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1722,12 +2008,12 @@
         <v>3</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>40. Veronese V, Traeger M, Oo ZM, Tun TT, Oo NN, Maung H, Hughes C, Pedrana A, Stoové M. HIV Incidence and Factors Associated with Testing Positive for HIV among Men Who Have Sex with Men and Transgender Women in Myanmar: Data from Community-based HIV Testing Services. Journal of the International AIDS Society. 2020;23(2). doi:10.1002/jia2.25454 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>40. Veronese V, Traeger M, Oo ZM, Tun TT, Oo NN, Maung H, Hughes C, Pedrana A, Stoové M. HIV Incidence and Factors Associated with Testing Positive for HIV among Men Who Have Sex with Men and Transgender Women in Myanmar: Data from Community-based HIV Testing Services. Journal of the International AIDS Society. 2020;23(2). doi:10.1002/jia2.25454. **[Link]( ). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1735,15 +2021,15 @@
         <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>41. **Traeger MW**, Cornelisse VJ, Asselin J, Price B, Roth NJ, Willcox J, Tee BK, Fairly CK, Chang CC, Armishaw J, Vujovic O, Penn M, Cundill P, Forgan-Smith G, Gall J, Pickett C, Lal L, Mak A, Spelman TD, Nguyen L, Murphy DA, Ryan KE, El-Hayek C, West M, Ruth S, Batrouney C, Lockwood JT, Hoy JF, Hellard ME, Stoové MA, Wright EJ. Association of HIV Pre-exposure Prophylaxis with Incidence of Sexually Transmitted Infections among Individuals at High Risk of HIV Infection. Journal of the American Medical Association. 2019;321(14):1380-1390. doi: 10.1001/jama.2019.2947 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>41. **Traeger MW**, Cornelisse VJ, Asselin J, Price B, Roth NJ, Willcox J, Tee BK, Fairly CK, Chang CC, Armishaw J, Vujovic O, Penn M, Cundill P, Forgan-Smith G, Gall J, Pickett C, Lal L, Mak A, Spelman TD, Nguyen L, Murphy DA, Ryan KE, El-Hayek C, West M, Ruth S, Batrouney C, Lockwood JT, Hoy JF, Hellard ME, Stoové MA, Wright EJ. Association of HIV Pre-exposure Prophylaxis with Incidence of Sexually Transmitted Infections among Individuals at High Risk of HIV Infection. Journal of the American Medical Association. 2019;321(14):1380-1390. doi: 10.1001/jama.2019.2947. **[Link]( ). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,15 +2037,15 @@
         <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>42. **Traeger MW**, Schroeder SE, Wright EJ, Hellard ME, Cornelisse VJ, Stoové MA. Effects of Pre-exposure Prophylaxis for the Prevention of Human Immunodeficiency Virus Infection on Sexual Risk Behavior in Men Who Have Sex with Men: A Systematic Review and Meta-analysis. Clinical Infectious Diseases. 2018;67(5):767-86. doi: 10.1093/cid/ciy182 . **[Link]( ). [PDF](/assets/papers/).**</v>
+        <v>42. **Traeger MW**, Schroeder SE, Wright EJ, Hellard ME, Cornelisse VJ, Stoové MA. Effects of Pre-exposure Prophylaxis for the Prevention of Human Immunodeficiency Virus Infection on Sexual Risk Behavior in Men Who Have Sex with Men: A Systematic Review and Meta-analysis. Clinical Infectious Diseases. 2018;67(5):767-86. doi: 10.1093/cid/ciy182. **[Link]( ). [PDF](/assets/papers/).**</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1907,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02F1DA3-FF52-574B-889A-EADAE9A6E722}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="F82" sqref="C82:F87"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE(A2,". ",B2)</f>
@@ -1937,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">CONCATENATE(A3,". ",B3)</f>
@@ -1949,7 +2235,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1961,7 +2247,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1973,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1985,7 +2271,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1997,7 +2283,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2009,7 +2295,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2021,7 +2307,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2033,7 +2319,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2045,7 +2331,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2057,7 +2343,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2069,7 +2355,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2081,7 +2367,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -2093,7 +2379,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2105,7 +2391,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2117,7 +2403,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2129,7 +2415,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2141,7 +2427,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2153,7 +2439,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2165,7 +2451,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2177,7 +2463,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2189,7 +2475,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2201,7 +2487,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2213,7 +2499,7 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2225,11 +2511,11 @@
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">26. 26. **Traeger M**, Asselin J, Ryan K, Doyle J, Harney B, Pedrana A, El-Hayek C, </v>
+        <v>26. **Traeger M**, Asselin J, Ryan K, Doyle J, Harney B, Pedrana A, El-Hayek C, Nguyen L, Roth N, Fairley C, Willcox J, Tee BK, Guy R, Wright E, Hellard M, Stoové. Adherence to Hepatitis C testing guidelines among Victorian gay and bisexual men using HIV pre-exposure prophylaxis. Australasian HIV&amp;AIDS and Sexual Health Conferences, Perth, Australia. 16-19 September 2019.</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2237,7 +2523,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2249,7 +2535,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2547,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2273,7 +2559,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2285,7 +2571,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2297,7 +2583,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2309,7 +2595,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -2321,7 +2607,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -2333,7 +2619,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -2345,7 +2631,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -2357,7 +2643,7 @@
         <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -2369,7 +2655,7 @@
         <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -2381,7 +2667,7 @@
         <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -2393,7 +2679,7 @@
         <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -2405,7 +2691,7 @@
         <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -2417,7 +2703,7 @@
         <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -2429,7 +2715,7 @@
         <v>46</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -2441,7 +2727,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -2453,7 +2739,7 @@
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -2465,7 +2751,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -2477,7 +2763,7 @@
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -2489,7 +2775,7 @@
         <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -2501,7 +2787,7 @@
         <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -2513,7 +2799,7 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -2525,7 +2811,7 @@
         <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -2537,7 +2823,7 @@
         <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -2549,7 +2835,7 @@
         <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -2561,7 +2847,7 @@
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -2573,7 +2859,7 @@
         <v>58</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -2585,7 +2871,7 @@
         <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -2597,7 +2883,7 @@
         <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -2609,7 +2895,7 @@
         <v>61</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2621,7 +2907,7 @@
         <v>62</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2633,7 +2919,7 @@
         <v>63</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2645,7 +2931,7 @@
         <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2657,7 +2943,7 @@
         <v>65</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2669,7 +2955,7 @@
         <v>66</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2681,7 +2967,7 @@
         <v>67</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2693,7 +2979,7 @@
         <v>68</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2705,7 +2991,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C80" si="1">CONCATENATE(A67,". ",B67)</f>
@@ -2717,7 +3003,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -2729,7 +3015,7 @@
         <v>71</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -2741,7 +3027,7 @@
         <v>72</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -2750,10 +3036,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -2762,10 +3048,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -2774,10 +3060,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -2786,10 +3072,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -2798,10 +3084,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -2810,10 +3096,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -2822,10 +3108,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -2834,10 +3120,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -2846,10 +3132,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -2861,7 +3147,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>

</xml_diff>